<commit_message>
Update dataframes & figures
</commit_message>
<xml_diff>
--- a/execution_time.xlsx
+++ b/execution_time.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tunopham/MyDocs/ESIEA_4A/common_core/system_programming/06_IPC/lab6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tunopham/MyDocs/ESIEA_4A/common_core/system_programming/06_IPC/lab6/lab6_streamlit_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F0FAE1-EAF1-1847-9DB5-5937559C2593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB8E158-CE5D-0642-A49C-AEFAA209CCF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{BA02B578-EE90-B74E-A7CD-0927BEFD2E02}"/>
+    <workbookView xWindow="69320" yWindow="-9280" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{BA02B578-EE90-B74E-A7CD-0927BEFD2E02}"/>
   </bookViews>
   <sheets>
     <sheet name="MACOS-M1PRO" sheetId="1" r:id="rId1"/>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D65CACD-0FB7-DE49-96D2-2D599A09E684}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection sqref="A1:B20"/>
+      <selection activeCell="B16" sqref="A2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +439,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>10.811323</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -447,7 +447,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>6.6500539999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -455,7 +455,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>4.9130419999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -463,7 +463,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>3.7476699999999998</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -471,7 +471,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>3.3565109999999998</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -479,7 +479,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>12</v>
+        <v>2.9822449999999998</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -487,7 +487,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>14</v>
+        <v>2.7423449999999998</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -495,7 +495,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>2.563434</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -503,7 +503,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>18</v>
+        <v>2.792875</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -511,7 +511,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>2.740008</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -519,7 +519,7 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>22</v>
+        <v>2.7973690000000002</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -527,7 +527,7 @@
         <v>30</v>
       </c>
       <c r="B13">
-        <v>24</v>
+        <v>2.63313</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -535,7 +535,7 @@
         <v>40</v>
       </c>
       <c r="B14">
-        <v>26</v>
+        <v>2.8548420000000001</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -543,7 +543,7 @@
         <v>50</v>
       </c>
       <c r="B15">
-        <v>28</v>
+        <v>2.7270539999999999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -551,39 +551,7 @@
         <v>100</v>
       </c>
       <c r="B16">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>200</v>
-      </c>
-      <c r="B17">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>300</v>
-      </c>
-      <c r="B18">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>500</v>
-      </c>
-      <c r="B19">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>1000</v>
-      </c>
-      <c r="B20">
-        <v>38</v>
+        <v>2.761927</v>
       </c>
     </row>
   </sheetData>
@@ -593,10 +561,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC656805-0217-4D40-92C6-C3416BD18F49}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,7 +582,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>17.208359000000002</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -622,7 +590,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>10.21893</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -630,7 +598,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>12</v>
+        <v>7.7816650000000003</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -638,7 +606,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>6.2256679999999998</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -646,7 +614,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>6.581353</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -654,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>24</v>
+        <v>5.8057499999999997</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -662,7 +630,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>28</v>
+        <v>5.3801819999999996</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -670,7 +638,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>32</v>
+        <v>4.8591629999999997</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -678,7 +646,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>36</v>
+        <v>5.3230870000000001</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -686,7 +654,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>40</v>
+        <v>5.2516540000000003</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -694,7 +662,7 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>44</v>
+        <v>5.243163</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -702,7 +670,7 @@
         <v>30</v>
       </c>
       <c r="B13">
-        <v>48</v>
+        <v>4.9566990000000004</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -710,7 +678,7 @@
         <v>40</v>
       </c>
       <c r="B14">
-        <v>52</v>
+        <v>5.4004570000000003</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -718,7 +686,7 @@
         <v>50</v>
       </c>
       <c r="B15">
-        <v>56</v>
+        <v>5.1228579999999999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -726,39 +694,7 @@
         <v>100</v>
       </c>
       <c r="B16">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>200</v>
-      </c>
-      <c r="B17">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>300</v>
-      </c>
-      <c r="B18">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>500</v>
-      </c>
-      <c r="B19">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>1000</v>
-      </c>
-      <c r="B20">
-        <v>76</v>
+        <v>5.2514940000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>